<commit_message>
adding hand descriptions to xml
</commit_message>
<xml_diff>
--- a/ReplaceIVTFFtoTEI.xlsx
+++ b/ReplaceIVTFFtoTEI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hadle\Documents\GitHub\voynichTEI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B44B3A-A8D3-4FA2-88E0-84A3C9C56912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE40EB56-A17F-4FE0-980B-8BE0B1B472FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9012" yWindow="216" windowWidth="14604" windowHeight="11952" xr2:uid="{DF9BB7F7-DEE6-4231-B8AE-192266D5BB45}"/>
+    <workbookView xWindow="2688" yWindow="912" windowWidth="7656" windowHeight="11952" xr2:uid="{DF9BB7F7-DEE6-4231-B8AE-192266D5BB45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="288">
   <si>
     <t>Voynich</t>
   </si>
@@ -474,9 +474,6 @@
   </si>
   <si>
     <t>\$L=B</t>
-  </si>
-  <si>
-    <t>Writing Hand Used</t>
   </si>
   <si>
     <t>\$H=1</t>
@@ -878,6 +875,33 @@
   </si>
   <si>
     <t>Comment Line</t>
+  </si>
+  <si>
+    <t>Scribe 1</t>
+  </si>
+  <si>
+    <t>Scribe 2</t>
+  </si>
+  <si>
+    <t>Scribe 3</t>
+  </si>
+  <si>
+    <t>Scribe 4</t>
+  </si>
+  <si>
+    <t>Scribe 5</t>
+  </si>
+  <si>
+    <t>Writing Hand Used (https://muse.jhu.edu/pub/56/article/754633/pdf) Page 7-8 (https://ceur-ws.org/Vol-3313/keynote2.pdf) Page 3</t>
+  </si>
+  <si>
+    <t>Language A</t>
+  </si>
+  <si>
+    <t>Language B</t>
+  </si>
+  <si>
+    <t>the first twelve lines were written by Scribe 2, the rest Scribe 3</t>
   </si>
 </sst>
 </file>
@@ -981,7 +1005,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -994,7 +1018,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1331,8 +1354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D110CFE0-76A4-4947-8E53-2D23B2B7842A}">
   <dimension ref="A1:K108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H57" workbookViewId="0">
-      <selection activeCell="K64" sqref="K64"/>
+    <sheetView tabSelected="1" topLeftCell="F74" workbookViewId="0">
+      <selection activeCell="I85" sqref="I85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1361,10 +1384,10 @@
         <v>45</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1381,10 +1404,10 @@
         <v>46</v>
       </c>
       <c r="J2" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1401,10 +1424,10 @@
         <v>7.5</v>
       </c>
       <c r="J3" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>176</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1427,10 +1450,10 @@
         <v>48</v>
       </c>
       <c r="J4" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>178</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1447,10 +1470,10 @@
         <v>1</v>
       </c>
       <c r="J5" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>180</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1473,10 +1496,10 @@
         <v>2</v>
       </c>
       <c r="J6" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="K6" s="4" t="s">
         <v>182</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1499,10 +1522,10 @@
         <v>3</v>
       </c>
       <c r="J7" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>184</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -1519,10 +1542,10 @@
         <v>4</v>
       </c>
       <c r="J8" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="K8" s="4" t="s">
         <v>186</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1539,10 +1562,10 @@
         <v>5</v>
       </c>
       <c r="J9" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="K9" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1573,10 +1596,10 @@
         <v>7</v>
       </c>
       <c r="J11" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1596,7 +1619,7 @@
         <v>93</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1613,10 +1636,10 @@
         <v>9</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1633,10 +1656,10 @@
         <v>10</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1653,10 +1676,10 @@
         <v>11</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1673,10 +1696,10 @@
         <v>12</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.3">
@@ -1693,10 +1716,10 @@
         <v>13</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="4:11" x14ac:dyDescent="0.3">
@@ -1713,10 +1736,10 @@
         <v>14</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.3">
@@ -1736,7 +1759,7 @@
         <v>92</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.3">
@@ -1753,10 +1776,10 @@
         <v>17</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.3">
@@ -1773,10 +1796,10 @@
         <v>19</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1793,10 +1816,10 @@
         <v>20</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1807,10 +1830,10 @@
         <v>187.5</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="4:11" x14ac:dyDescent="0.3">
@@ -1827,10 +1850,10 @@
         <v>94</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="4:11" x14ac:dyDescent="0.3">
@@ -1847,10 +1870,10 @@
         <v>1</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" spans="4:11" x14ac:dyDescent="0.3">
@@ -1867,10 +1890,10 @@
         <v>2</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="4:11" x14ac:dyDescent="0.3">
@@ -1887,10 +1910,10 @@
         <v>3</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="28" spans="4:11" x14ac:dyDescent="0.3">
@@ -1907,10 +1930,10 @@
         <v>4</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="29" spans="4:11" x14ac:dyDescent="0.3">
@@ -1927,10 +1950,10 @@
         <v>5</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="30" spans="4:11" x14ac:dyDescent="0.3">
@@ -1950,7 +1973,7 @@
         <v>91</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="31" spans="4:11" x14ac:dyDescent="0.3">
@@ -1967,10 +1990,10 @@
         <v>7</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="4:11" x14ac:dyDescent="0.3">
@@ -1987,10 +2010,10 @@
         <v>8</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="33" spans="4:11" x14ac:dyDescent="0.3">
@@ -2007,10 +2030,10 @@
         <v>9</v>
       </c>
       <c r="J33" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="34" spans="4:11" x14ac:dyDescent="0.3">
@@ -2027,10 +2050,10 @@
         <v>10</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="35" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2047,10 +2070,10 @@
         <v>11</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="36" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2081,7 +2104,7 @@
         <v>13</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K37" s="2"/>
     </row>
@@ -2099,10 +2122,10 @@
         <v>14</v>
       </c>
       <c r="J38" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="39" spans="4:11" x14ac:dyDescent="0.3">
@@ -2119,10 +2142,10 @@
         <v>15</v>
       </c>
       <c r="J39" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="40" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2139,10 +2162,10 @@
         <v>16</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="41" spans="4:11" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2153,10 +2176,10 @@
         <v>17</v>
       </c>
       <c r="J41" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K41" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="42" spans="4:11" x14ac:dyDescent="0.3">
@@ -2170,7 +2193,7 @@
         <v>24</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="43" spans="4:11" x14ac:dyDescent="0.3">
@@ -2181,10 +2204,10 @@
         <v>19</v>
       </c>
       <c r="J43" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="44" spans="4:11" x14ac:dyDescent="0.3">
@@ -2195,10 +2218,10 @@
         <v>20</v>
       </c>
       <c r="J44" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="45" spans="4:11" x14ac:dyDescent="0.3">
@@ -2209,10 +2232,10 @@
         <v>21</v>
       </c>
       <c r="J45" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="46" spans="4:11" x14ac:dyDescent="0.3">
@@ -2223,10 +2246,10 @@
         <v>22</v>
       </c>
       <c r="J46" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="47" spans="4:11" x14ac:dyDescent="0.3">
@@ -2237,10 +2260,10 @@
         <v>23</v>
       </c>
       <c r="J47" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="K47" s="4" t="s">
         <v>258</v>
-      </c>
-      <c r="K47" s="4" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="48" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2251,18 +2274,18 @@
         <v>24</v>
       </c>
       <c r="J48" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="49" spans="7:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J49" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="50" spans="7:11" x14ac:dyDescent="0.3">
@@ -2273,10 +2296,10 @@
         <v>103</v>
       </c>
       <c r="J50" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="51" spans="7:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2285,10 +2308,10 @@
       </c>
       <c r="H51" s="4"/>
       <c r="J51" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K51" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="52" spans="7:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2303,7 +2326,7 @@
       </c>
       <c r="H53" s="4"/>
       <c r="J53" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K53" s="2"/>
     </row>
@@ -2313,10 +2336,10 @@
       </c>
       <c r="H54" s="4"/>
       <c r="J54" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="55" spans="7:11" x14ac:dyDescent="0.3">
@@ -2325,10 +2348,10 @@
       </c>
       <c r="H55" s="4"/>
       <c r="J55" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="56" spans="7:11" x14ac:dyDescent="0.3">
@@ -2337,10 +2360,10 @@
       </c>
       <c r="H56" s="4"/>
       <c r="J56" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="57" spans="7:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -2349,10 +2372,10 @@
       </c>
       <c r="H57" s="4"/>
       <c r="J57" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K57" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="58" spans="7:11" x14ac:dyDescent="0.3">
@@ -2361,10 +2384,10 @@
       </c>
       <c r="H58" s="4"/>
       <c r="J58" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K58" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="59" spans="7:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2373,10 +2396,10 @@
       </c>
       <c r="H59" s="4"/>
       <c r="J59" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K59" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="60" spans="7:11" x14ac:dyDescent="0.3">
@@ -2384,11 +2407,11 @@
         <v>113</v>
       </c>
       <c r="H60" s="4"/>
-      <c r="J60" s="10" t="s">
+      <c r="J60" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="K60" t="s">
         <v>274</v>
-      </c>
-      <c r="K60" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="61" spans="7:11" x14ac:dyDescent="0.3">
@@ -2396,11 +2419,11 @@
         <v>114</v>
       </c>
       <c r="H61" s="4"/>
-      <c r="J61" s="10" t="s">
+      <c r="J61" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="K61" t="s">
         <v>276</v>
-      </c>
-      <c r="K61" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="62" spans="7:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2411,10 +2434,10 @@
     </row>
     <row r="63" spans="7:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J63" t="s">
+        <v>277</v>
+      </c>
+      <c r="K63" t="s">
         <v>278</v>
-      </c>
-      <c r="K63" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="64" spans="7:11" x14ac:dyDescent="0.3">
@@ -2559,155 +2582,171 @@
       <c r="G83" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="H83" s="4"/>
+      <c r="H83" s="4" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="84" spans="7:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G84" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="H84" s="6"/>
+      <c r="H84" s="6" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="85" spans="7:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="86" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G86" s="1" t="s">
-        <v>146</v>
+        <v>284</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="87" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G87" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="H87" s="4"/>
+        <v>146</v>
+      </c>
+      <c r="H87" s="4" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="88" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G88" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="H88" s="4"/>
+        <v>147</v>
+      </c>
+      <c r="H88" s="4" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="89" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G89" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="H89" s="4"/>
+        <v>148</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="90" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G90" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="H90" s="4"/>
+        <v>149</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="91" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G91" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H91" s="4"/>
+        <v>150</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="92" spans="7:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G92" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="H92" s="6"/>
+        <v>151</v>
+      </c>
+      <c r="H92" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="93" spans="7:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="94" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G94" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="95" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G95" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H95" s="4"/>
     </row>
     <row r="96" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G96" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H96" s="4"/>
     </row>
     <row r="97" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G97" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H97" s="4"/>
     </row>
     <row r="98" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G98" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H98" s="4"/>
     </row>
     <row r="99" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G99" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H99" s="4"/>
     </row>
     <row r="100" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G100" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H100" s="4"/>
     </row>
     <row r="101" spans="7:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G101" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H101" s="6"/>
     </row>
     <row r="102" spans="7:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="103" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G103" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H103" s="2"/>
     </row>
     <row r="104" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G104" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H104" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="105" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G105" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H105" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="106" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G106" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H106" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="107" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G107" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H107" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="108" spans="7:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G108" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H108" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>